<commit_message>
comment some test cases
</commit_message>
<xml_diff>
--- a/data/orangehrmData.xlsx
+++ b/data/orangehrmData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26202"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{173DE68F-6E17-495E-AE19-4E4DF21363B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{588F2F6E-C7C0-42E8-9107-83FEB3AFA3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,6 +339,15 @@
     <t>2023-05-02</t>
   </si>
   <si>
+    <t>Cecil Bonaparte</t>
+  </si>
+  <si>
+    <t>2023-04-06</t>
+  </si>
+  <si>
+    <t>2023-04-02</t>
+  </si>
+  <si>
     <t>Odis Adalwin</t>
   </si>
   <si>
@@ -349,15 +358,6 @@
   </si>
   <si>
     <t>2023-02-02</t>
-  </si>
-  <si>
-    <t>Cecil Bonaparte</t>
-  </si>
-  <si>
-    <t>2023-04-06</t>
-  </si>
-  <si>
-    <t>2023-04-02</t>
   </si>
   <si>
     <t>2023-02-05</t>
@@ -1022,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2A7B0-BEF2-4260-8257-31FC2B7FF305}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1182,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4A3639-CCA0-4A94-AD00-8D71C962DA75}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1240,27 +1240,27 @@
       <c r="A4" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1269,10 +1269,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>109</v>
@@ -1289,7 +1289,7 @@
         <v>109</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75">
@@ -1317,7 +1317,7 @@
         <v>116</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>